<commit_message>
Update Login Gmail python
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="122">
   <si>
     <t>C:\Users\Admin\Desktop\HCVIP - 3\ChromeProfile\ChromeProfile\ChromeProfile - 1</t>
   </si>
@@ -388,6 +388,9 @@
   </si>
   <si>
     <t>0dalfatraktor8971@web.de</t>
+  </si>
+  <si>
+    <t>Login Thành Công</t>
   </si>
 </sst>
 </file>
@@ -752,7 +755,7 @@
   <dimension ref="A1:O48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,6 +780,9 @@
       <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="C1" t="s">
+        <v>121</v>
+      </c>
       <c r="F1" t="s">
         <v>106</v>
       </c>
@@ -1421,6 +1427,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>